<commit_message>
updated data dictionary (long form, rather than columns for scale)
</commit_message>
<xml_diff>
--- a/process/configuration/assets/output_data_dictionary.xlsx
+++ b/process/configuration/assets/output_data_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/process/configuration/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6C2A9E9-1E3C-4AE2-AFDC-D6EEE11C58B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{A6C2A9E9-1E3C-4AE2-AFDC-D6EEE11C58B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12331DEC-CA0C-4018-B54D-0029A7CF85BD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6A734B74-6998-4CFA-84B5-68C9F1C50A0B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6A734B74-6998-4CFA-84B5-68C9F1C50A0B}"/>
   </bookViews>
   <sheets>
     <sheet name="output_data_dictionary" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="90">
   <si>
     <t>Continent</t>
   </si>
@@ -125,27 +125,15 @@
     <t>pop_pct_access_500m_pt_any_score</t>
   </si>
   <si>
-    <t>Average walkable neighbourhood poulation density (population weighted) *</t>
-  </si>
-  <si>
     <t>pop_nh_pop_density</t>
   </si>
   <si>
-    <t>Average walkable neighbourhood intersection density (population weighted) *</t>
-  </si>
-  <si>
     <t>pop_nh_intersection_density</t>
   </si>
   <si>
-    <t>Average daily living score (population weighted) *</t>
-  </si>
-  <si>
     <t>pop_daily_living</t>
   </si>
   <si>
-    <t>Average walkability (population weighted) *</t>
-  </si>
-  <si>
     <t>pop_walkability</t>
   </si>
   <si>
@@ -176,18 +164,6 @@
     <t>2-letter country code</t>
   </si>
   <si>
-    <t>Type of measure</t>
-  </si>
-  <si>
-    <t>Grid data</t>
-  </si>
-  <si>
-    <t>City data</t>
-  </si>
-  <si>
-    <t>study_region</t>
-  </si>
-  <si>
     <t>Study region</t>
   </si>
   <si>
@@ -203,9 +179,6 @@
     <t>Intersection count (following consolidation based on intersection tolerance parameter in region configuration)</t>
   </si>
   <si>
-    <t>Linked urban covariates (e.g. estimates for 2015 from GHSL UCDB on air pollution)</t>
-  </si>
-  <si>
     <t>Sample points used in this analysis (generated along pedestrian network for populated grid areas)</t>
   </si>
   <si>
@@ -218,36 +191,6 @@
     <t>Analytical statistic</t>
   </si>
   <si>
-    <t>Access  (for city, population percentage /100; for grid, an access score /1) within 500 metres to:</t>
-  </si>
-  <si>
-    <t>fresh food market / supermarket (source: OpenStreetMap or custom)</t>
-  </si>
-  <si>
-    <t>convenience store (source: OpenStreetMap or custom)</t>
-  </si>
-  <si>
-    <t>public transport (source: OpenStreetMap or custom)</t>
-  </si>
-  <si>
-    <t>any public open space (source: OpenStreetMap)</t>
-  </si>
-  <si>
-    <t>public open space larger than 1.5 hectares (source: OpenStreetMap)</t>
-  </si>
-  <si>
-    <t>public transport (source: GTFS)</t>
-  </si>
-  <si>
-    <t>public transport with average daytime weekday service frequency of 30 minutes or better (source: GTFS)</t>
-  </si>
-  <si>
-    <t>public transport with average daytime weekday service frequency of 20 minutes or better (source: GTFS)</t>
-  </si>
-  <si>
-    <t>any public transport stop (source: GTFS or OpenStreetMap/custom)</t>
-  </si>
-  <si>
     <t>access_500m_fresh_food_market_score</t>
   </si>
   <si>
@@ -278,14 +221,98 @@
     <t>Indicator estimates</t>
   </si>
   <si>
-    <t>Measure or data item description</t>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Scale</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>city, grid</t>
+  </si>
+  <si>
+    <t>Score (/1) for access within 500 m to a  fresh food market / supermarket (source: OpenStreetMap or custom)</t>
+  </si>
+  <si>
+    <t>grid</t>
+  </si>
+  <si>
+    <t>Score (/1) for access within 500 m to a  convenience store (source: OpenStreetMap or custom)</t>
+  </si>
+  <si>
+    <t>Score (/1) for access within 500 m to a  public transport (source: OpenStreetMap or custom)</t>
+  </si>
+  <si>
+    <t>Score (/1) for access within 500 m to a  any public open space (source: OpenStreetMap)</t>
+  </si>
+  <si>
+    <t>Score (/1) for access within 500 m to a  public open space larger than 1.5 hectares (source: OpenStreetMap)</t>
+  </si>
+  <si>
+    <t>Score (/1) for access within 500 m to a  public transport (source: GTFS)</t>
+  </si>
+  <si>
+    <t>Score (/1) for access within 500 m to a  public transport with average daytime weekday service frequency of 30 minutes or better (source: GTFS)</t>
+  </si>
+  <si>
+    <t>Score (/1) for access within 500 m to a  public transport with average daytime weekday service frequency of 20 minutes or better (source: GTFS)</t>
+  </si>
+  <si>
+    <t>Score (/1) for access within 500 m to a  any public transport stop (source: GTFS or OpenStreetMap/custom)</t>
+  </si>
+  <si>
+    <t>Percentage of population with access within 500 m to a  fresh food market / supermarket (source: OpenStreetMap or custom)</t>
+  </si>
+  <si>
+    <t>Percentage of population with access within 500 m to a  convenience store (source: OpenStreetMap or custom)</t>
+  </si>
+  <si>
+    <t>Percentage of population with access within 500 m to a  public transport (source: OpenStreetMap or custom)</t>
+  </si>
+  <si>
+    <t>Percentage of population with access within 500 m to a  any public open space (source: OpenStreetMap)</t>
+  </si>
+  <si>
+    <t>Percentage of population with access within 500 m to a  public open space larger than 1.5 hectares (source: OpenStreetMap)</t>
+  </si>
+  <si>
+    <t>Percentage of population with access within 500 m to a  public transport (source: GTFS)</t>
+  </si>
+  <si>
+    <t>Percentage of population with access within 500 m to a  public transport with average daytime weekday service frequency of 30 minutes or better (source: GTFS)</t>
+  </si>
+  <si>
+    <t>Percentage of population with access within 500 m to a  public transport with average daytime weekday service frequency of 20 minutes or better (source: GTFS)</t>
+  </si>
+  <si>
+    <t>Percentage of population with access within 500 m to a  any public transport stop (source: GTFS or OpenStreetMap/custom)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average walkable neighbourhood poulation density (population weighted) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average walkable neighbourhood intersection density (population weighted) </t>
+  </si>
+  <si>
+    <t>Average daily living score (population weighted)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average walkability (population weighted) </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,14 +335,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -325,7 +344,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -375,29 +394,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -417,27 +418,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -753,10 +738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3379ABC2-E28B-4FB4-ABAD-BCC004EC2FB1}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -769,21 +754,21 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -792,12 +777,12 @@
         <v>0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>0</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>1</v>
@@ -806,68 +791,68 @@
         <v>1</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>1</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>6</v>
@@ -876,26 +861,26 @@
         <v>7</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>9</v>
@@ -904,329 +889,442 @@
         <v>10</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
+      <c r="A11" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="B11" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+        <v>11</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>11</v>
+        <v>49</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>13</v>
+        <v>49</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>15</v>
+        <v>49</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>17</v>
+        <v>50</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="A17" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>63</v>
+        <v>60</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>64</v>
+        <v>60</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>73</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>65</v>
+        <v>60</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>66</v>
+        <v>60</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>75</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>67</v>
+        <v>60</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>68</v>
+        <v>60</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>69</v>
+        <v>60</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>29</v>
-      </c>
       <c r="C27" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" s="6"/>
+        <v>22</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28" s="6"/>
+        <v>23</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D29" s="6"/>
+        <v>24</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D30" s="6"/>
+        <v>25</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>44</v>
+      <c r="A34" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="10"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
+      <c r="A35" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>66</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated gui app to work with new region checks
</commit_message>
<xml_diff>
--- a/process/configuration/assets/output_data_dictionary.xlsx
+++ b/process/configuration/assets/output_data_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/process/configuration/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{A6C2A9E9-1E3C-4AE2-AFDC-D6EEE11C58B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12331DEC-CA0C-4018-B54D-0029A7CF85BD}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{A6C2A9E9-1E3C-4AE2-AFDC-D6EEE11C58B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8368BD0-BB42-4C72-A605-72CBBBA31FED}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6A734B74-6998-4CFA-84B5-68C9F1C50A0B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6A734B74-6998-4CFA-84B5-68C9F1C50A0B}"/>
   </bookViews>
   <sheets>
     <sheet name="output_data_dictionary" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="98">
   <si>
     <t>Continent</t>
   </si>
@@ -47,9 +47,6 @@
     <t>ISO 3166-1 alpha-2</t>
   </si>
   <si>
-    <t>City</t>
-  </si>
-  <si>
     <t>Area (sqkm)</t>
   </si>
   <si>
@@ -306,6 +303,33 @@
   </si>
   <si>
     <t xml:space="preserve">Average walkability (population weighted) </t>
+  </si>
+  <si>
+    <t>study_region</t>
+  </si>
+  <si>
+    <t>The average elevation estimated within the spatial domain of the Urban Centre, and expressed in metres above sea level (MASL) (EORC &amp; JAXA, 2017).</t>
+  </si>
+  <si>
+    <t>EL_AV_ALS</t>
+  </si>
+  <si>
+    <t>Semi-colon separated list of names of Köppen-Geiger climate classes, intersecting with the spatial domain of the Urban Centre (1986-2010) (Rubel et al., 2017).</t>
+  </si>
+  <si>
+    <t>E_KG_NM_LST</t>
+  </si>
+  <si>
+    <t>Average temperature calculated from annual average estimates for time interval centred on the year 2015 (the interval spans from 2012 to 2015) within the spatial domain of the Urban Centre, and expressed in Celsius degrees (°C) (Harris et al., 2014).</t>
+  </si>
+  <si>
+    <t>E_WR_T_14</t>
+  </si>
+  <si>
+    <t>Average precipitations calculated from annual average estimates for time interval centred on the year 2015 (the interval spans from 2012 to 2015) within the spatial domain of the Urban Centre; and expressed in millimetres (mm), the amount of rain per square meter in one hour) (Harris et al., 2014).</t>
+  </si>
+  <si>
+    <t>E_WR_P_14</t>
   </si>
 </sst>
 </file>
@@ -738,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3379ABC2-E28B-4FB4-ABAD-BCC004EC2FB1}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -754,21 +778,21 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -777,12 +801,12 @@
         <v>0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>1</v>
@@ -791,539 +815,595 @@
         <v>1</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>3</v>
+        <v>89</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>7</v>
-      </c>
       <c r="D8" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>10</v>
-      </c>
       <c r="D10" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="D11" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>14</v>
-      </c>
       <c r="D12" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>16</v>
-      </c>
       <c r="D13" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="D14" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>19</v>
+        <v>91</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>52</v>
+        <v>95</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>70</v>
+        <v>96</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>53</v>
+        <v>97</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>35</v>
+        <v>86</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B40" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="D44" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D40" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B41" s="7" t="s">
+      <c r="C45" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>66</v>
+      <c r="D45" s="8" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
addresses #409, adding option to view and interact with spatial indicator choropleth map for analysed regions in the GHSCI web app
</commit_message>
<xml_diff>
--- a/process/configuration/assets/output_data_dictionary.xlsx
+++ b/process/configuration/assets/output_data_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/process/configuration/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{A6C2A9E9-1E3C-4AE2-AFDC-D6EEE11C58B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8368BD0-BB42-4C72-A605-72CBBBA31FED}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{A6C2A9E9-1E3C-4AE2-AFDC-D6EEE11C58B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BA39DA8-4667-432A-9393-65BB66CE92A0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6A734B74-6998-4CFA-84B5-68C9F1C50A0B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6A734B74-6998-4CFA-84B5-68C9F1C50A0B}"/>
   </bookViews>
   <sheets>
     <sheet name="output_data_dictionary" sheetId="1" r:id="rId1"/>
@@ -236,63 +236,9 @@
     <t>city, grid</t>
   </si>
   <si>
-    <t>Score (/1) for access within 500 m to a  fresh food market / supermarket (source: OpenStreetMap or custom)</t>
-  </si>
-  <si>
     <t>grid</t>
   </si>
   <si>
-    <t>Score (/1) for access within 500 m to a  convenience store (source: OpenStreetMap or custom)</t>
-  </si>
-  <si>
-    <t>Score (/1) for access within 500 m to a  public transport (source: OpenStreetMap or custom)</t>
-  </si>
-  <si>
-    <t>Score (/1) for access within 500 m to a  any public open space (source: OpenStreetMap)</t>
-  </si>
-  <si>
-    <t>Score (/1) for access within 500 m to a  public open space larger than 1.5 hectares (source: OpenStreetMap)</t>
-  </si>
-  <si>
-    <t>Score (/1) for access within 500 m to a  public transport (source: GTFS)</t>
-  </si>
-  <si>
-    <t>Score (/1) for access within 500 m to a  public transport with average daytime weekday service frequency of 30 minutes or better (source: GTFS)</t>
-  </si>
-  <si>
-    <t>Score (/1) for access within 500 m to a  public transport with average daytime weekday service frequency of 20 minutes or better (source: GTFS)</t>
-  </si>
-  <si>
-    <t>Score (/1) for access within 500 m to a  any public transport stop (source: GTFS or OpenStreetMap/custom)</t>
-  </si>
-  <si>
-    <t>Percentage of population with access within 500 m to a  fresh food market / supermarket (source: OpenStreetMap or custom)</t>
-  </si>
-  <si>
-    <t>Percentage of population with access within 500 m to a  convenience store (source: OpenStreetMap or custom)</t>
-  </si>
-  <si>
-    <t>Percentage of population with access within 500 m to a  public transport (source: OpenStreetMap or custom)</t>
-  </si>
-  <si>
-    <t>Percentage of population with access within 500 m to a  any public open space (source: OpenStreetMap)</t>
-  </si>
-  <si>
-    <t>Percentage of population with access within 500 m to a  public open space larger than 1.5 hectares (source: OpenStreetMap)</t>
-  </si>
-  <si>
-    <t>Percentage of population with access within 500 m to a  public transport (source: GTFS)</t>
-  </si>
-  <si>
-    <t>Percentage of population with access within 500 m to a  public transport with average daytime weekday service frequency of 30 minutes or better (source: GTFS)</t>
-  </si>
-  <si>
-    <t>Percentage of population with access within 500 m to a  public transport with average daytime weekday service frequency of 20 minutes or better (source: GTFS)</t>
-  </si>
-  <si>
-    <t>Percentage of population with access within 500 m to a  any public transport stop (source: GTFS or OpenStreetMap/custom)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Average walkable neighbourhood poulation density (population weighted) </t>
   </si>
   <si>
@@ -330,6 +276,60 @@
   </si>
   <si>
     <t>E_WR_P_14</t>
+  </si>
+  <si>
+    <t>Score (/1) for access within 500 m to a fresh food market / supermarket (source: OpenStreetMap or custom)</t>
+  </si>
+  <si>
+    <t>Score (/1) for access within 500 m to a convenience store (source: OpenStreetMap or custom)</t>
+  </si>
+  <si>
+    <t>Score (/1) for access within 500 m to public transport (source: OpenStreetMap or custom)</t>
+  </si>
+  <si>
+    <t>Score (/1) for access within 500 m to any public open space (source: OpenStreetMap)</t>
+  </si>
+  <si>
+    <t>Score (/1) for access within 500 m to a public open space larger than 1.5 hectares (source: OpenStreetMap)</t>
+  </si>
+  <si>
+    <t>Score (/1) for access within 500 m to public transport (source: GTFS)</t>
+  </si>
+  <si>
+    <t>Score (/1) for access within 500 m to public transport with average daytime weekday service frequency of 30 minutes or better (source: GTFS)</t>
+  </si>
+  <si>
+    <t>Score (/1) for access within 500 m to public transport with average daytime weekday service frequency of 20 minutes or better (source: GTFS)</t>
+  </si>
+  <si>
+    <t>Score (/1) for access within 500 m to any public transport stop (source: GTFS or OpenStreetMap/custom)</t>
+  </si>
+  <si>
+    <t>Percentage of population with access within 500 m to a fresh food market / supermarket (source: OpenStreetMap or custom)</t>
+  </si>
+  <si>
+    <t>Percentage of population with access within 500 m to a convenience store (source: OpenStreetMap or custom)</t>
+  </si>
+  <si>
+    <t>Percentage of population with access within 500 m to public transport (source: OpenStreetMap or custom)</t>
+  </si>
+  <si>
+    <t>Percentage of population with access within 500 m to any public open space (source: OpenStreetMap)</t>
+  </si>
+  <si>
+    <t>Percentage of population with access within 500 m to public open space larger than 1.5 hectares (source: OpenStreetMap)</t>
+  </si>
+  <si>
+    <t>Percentage of population with access within 500 m to public transport (source: GTFS)</t>
+  </si>
+  <si>
+    <t>Percentage of population with access within 500 m to public transport with average daytime weekday service frequency of 30 minutes or better (source: GTFS)</t>
+  </si>
+  <si>
+    <t>Percentage of population with access within 500 m to public transport with average daytime weekday service frequency of 20 minutes or better (source: GTFS)</t>
+  </si>
+  <si>
+    <t>Percentage of population with access within 500 m to any public transport stop (source: GTFS or OpenStreetMap/custom)</t>
   </si>
 </sst>
 </file>
@@ -466,9 +466,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -506,7 +506,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -612,7 +612,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -754,7 +754,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -764,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3379ABC2-E28B-4FB4-ABAD-BCC004EC2FB1}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -840,7 +840,7 @@
         <v>41</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>65</v>
@@ -977,10 +977,10 @@
         <v>48</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>64</v>
@@ -991,10 +991,10 @@
         <v>48</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>64</v>
@@ -1005,10 +1005,10 @@
         <v>48</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>64</v>
@@ -1019,10 +1019,10 @@
         <v>48</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>64</v>
@@ -1047,13 +1047,13 @@
         <v>59</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>50</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1061,13 +1061,13 @@
         <v>59</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>51</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1075,13 +1075,13 @@
         <v>59</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1089,13 +1089,13 @@
         <v>59</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>53</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1103,13 +1103,13 @@
         <v>59</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>54</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1117,13 +1117,13 @@
         <v>59</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>55</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1131,13 +1131,13 @@
         <v>59</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>56</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1145,13 +1145,13 @@
         <v>59</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1159,13 +1159,13 @@
         <v>59</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>58</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1173,7 +1173,7 @@
         <v>59</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>19</v>
@@ -1187,7 +1187,7 @@
         <v>59</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>20</v>
@@ -1201,7 +1201,7 @@
         <v>59</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>21</v>
@@ -1215,7 +1215,7 @@
         <v>59</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>22</v>
@@ -1229,7 +1229,7 @@
         <v>59</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>23</v>
@@ -1243,7 +1243,7 @@
         <v>59</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>24</v>
@@ -1257,7 +1257,7 @@
         <v>59</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>25</v>
@@ -1271,7 +1271,7 @@
         <v>59</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>26</v>
@@ -1285,7 +1285,7 @@
         <v>59</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>27</v>
@@ -1299,7 +1299,7 @@
         <v>59</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>28</v>
@@ -1313,7 +1313,7 @@
         <v>59</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>29</v>
@@ -1327,7 +1327,7 @@
         <v>59</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>30</v>
@@ -1341,7 +1341,7 @@
         <v>59</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
updated output data dictionary for #572
</commit_message>
<xml_diff>
--- a/process/configuration/assets/output_data_dictionary.xlsx
+++ b/process/configuration/assets/output_data_dictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/process/configuration/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\repos\global-indicators\process\configuration\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{A6C2A9E9-1E3C-4AE2-AFDC-D6EEE11C58B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BA39DA8-4667-432A-9393-65BB66CE92A0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F663036E-A009-4B3E-AF64-5D6042ECFDF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6A734B74-6998-4CFA-84B5-68C9F1C50A0B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="101">
   <si>
     <t>Continent</t>
   </si>
@@ -330,6 +330,15 @@
   </si>
   <si>
     <t>Percentage of population with access within 500 m to any public transport stop (source: GTFS or OpenStreetMap/custom)</t>
+  </si>
+  <si>
+    <t>Score (/1) for access within 500m to a large public green space of at least 1 hectare in size (source: OpenStreetMap, Google Earth Engine)</t>
+  </si>
+  <si>
+    <t>access_500m_large_public_green_space_score</t>
+  </si>
+  <si>
+    <t>Percentage of population with access within 500 m to large public green space of at least 1 hectare in size (source: OpenStreetMap, Google Earth Engine)</t>
   </si>
 </sst>
 </file>
@@ -762,10 +771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3379ABC2-E28B-4FB4-ABAD-BCC004EC2FB1}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1117,10 +1126,10 @@
         <v>59</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>66</v>
@@ -1131,10 +1140,10 @@
         <v>59</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>66</v>
@@ -1145,10 +1154,10 @@
         <v>59</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>66</v>
@@ -1159,10 +1168,10 @@
         <v>59</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>66</v>
@@ -1173,13 +1182,13 @@
         <v>59</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1187,10 +1196,10 @@
         <v>59</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>64</v>
@@ -1201,10 +1210,10 @@
         <v>59</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>64</v>
@@ -1215,10 +1224,10 @@
         <v>59</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>64</v>
@@ -1229,180 +1238,208 @@
         <v>59</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C34" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D33" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B34" s="5" t="s">
+      <c r="D34" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C36" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B35" s="5" t="s">
+      <c r="D36" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C37" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B36" s="5" t="s">
+      <c r="D37" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C38" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D36" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B37" s="5" t="s">
+      <c r="D38" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C39" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D37" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B38" s="5" t="s">
+      <c r="D39" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C40" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D38" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B39" s="5" t="s">
+      <c r="D40" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C41" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D39" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B40" s="5" t="s">
+      <c r="D41" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C42" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D40" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B41" s="5" t="s">
+      <c r="D42" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C43" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D41" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B42" s="5" t="s">
+      <c r="D43" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C44" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B45" s="7" t="s">
+    <row r="45" spans="1:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C47" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D47" s="8" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>